<commit_message>
Add room temperature read from analog thermistor
</commit_message>
<xml_diff>
--- a/Planning (personal - in finnish).xlsx
+++ b/Planning (personal - in finnish).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tiedostot\GitHub\cottageHeater\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="22035" windowHeight="8265" activeTab="1"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Ohjelmointi" sheetId="2" r:id="rId2"/>
     <sheet name="Taul3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -153,7 +158,7 @@
     <t>on/off/disable</t>
   </si>
   <si>
-    <t>tavoitelämpötila(0 - 25)</t>
+    <t>tavoitelämpötila(0 - 25,4)</t>
   </si>
 </sst>
 </file>
@@ -475,6 +480,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -982,7 +990,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1017,7 +1025,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1443,7 +1451,7 @@
   <dimension ref="A5:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>